<commit_message>
added kdm extractor into the project for further development
</commit_message>
<xml_diff>
--- a/data/UseCaseWeighting/datasets_5_15/data_points_accuracy.xlsx
+++ b/data/UseCaseWeighting/datasets_5_15/data_points_accuracy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="49">
   <si>
     <t>Data_Set</t>
   </si>
@@ -131,13 +131,49 @@
   </si>
   <si>
     <t>t-value</t>
+  </si>
+  <si>
+    <t>t-Test: Two-Sample Assuming Unequal Variances</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Hypothesized Mean Difference</t>
+  </si>
+  <si>
+    <t>df</t>
+  </si>
+  <si>
+    <t>t Stat</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) one-tail</t>
+  </si>
+  <si>
+    <t>t Critical one-tail</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) two-tail</t>
+  </si>
+  <si>
+    <t>t Critical two-tail</t>
+  </si>
+  <si>
+    <t>t-critical</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,6 +304,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -454,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -569,6 +613,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -614,8 +678,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -937,23 +1006,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:AA60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" customWidth="1"/>
     <col min="9" max="9" width="17.5703125" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="20" max="20" width="18.7109375" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="26" max="26" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -991,7 +1065,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1008,7 +1082,7 @@
         <v>0.71447470000000002</v>
       </c>
       <c r="F2">
-        <v>0.19644865400312733</v>
+        <v>0.196448654003127</v>
       </c>
       <c r="G2">
         <v>0.44166670000000002</v>
@@ -1029,7 +1103,7 @@
         <v>7.5000000740740966E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1067,7 +1141,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1105,7 +1179,7 @@
         <v>6.8098064139197348E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1142,8 +1216,14 @@
       <c r="L5">
         <v>8.611111397849483E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1181,7 +1261,7 @@
         <v>2.1821782477062523E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1218,8 +1298,22 @@
       <c r="L7">
         <v>4.6569533515100771E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T7" s="3"/>
+      <c r="U7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1256,8 +1350,26 @@
       <c r="L8">
         <v>4.6569533515100771E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="1">
+        <v>0.71447469200000002</v>
+      </c>
+      <c r="V8" s="1">
+        <v>0.883476598</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>0.49166665999999992</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0.33333332999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1294,8 +1406,26 @@
       <c r="L9">
         <v>4.4896104995469761E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.38592073659640441</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0.268117713813674</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>0.10254630111111165</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>8.9506175308642327E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1332,8 +1462,26 @@
       <c r="L10">
         <v>5.425935235089957E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U10" s="1">
+        <v>10</v>
+      </c>
+      <c r="V10" s="1">
+        <v>10</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>10</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1370,8 +1518,22 @@
       <c r="L11">
         <v>3.8173395732912029E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="U11" s="1">
+        <v>0</v>
+      </c>
+      <c r="V11" s="1"/>
+      <c r="Y11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -1408,8 +1570,22 @@
       <c r="L12">
         <v>3.8972096679025112E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="U12" s="1">
+        <v>17</v>
+      </c>
+      <c r="V12" s="1"/>
+      <c r="Y12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z12" s="1">
+        <v>18</v>
+      </c>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1446,9 +1622,54 @@
       <c r="L13">
         <v>5.7455169198194433E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="U13" s="1">
+        <v>-0.66083032186369195</v>
+      </c>
+      <c r="V13" s="1"/>
+      <c r="Y13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z13" s="1">
+        <v>1.1425162611450843</v>
+      </c>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="T14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U14" s="1">
+        <v>0.25878853949538672</v>
+      </c>
+      <c r="V14" s="1"/>
+      <c r="Y14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z14" s="1">
+        <v>0.13410480699317756</v>
+      </c>
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="T15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="U15" s="1">
+        <v>1.7396067260750732</v>
+      </c>
+      <c r="V15" s="1"/>
+      <c r="Y15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>1.7340636066175394</v>
+      </c>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1500,8 +1721,22 @@
       <c r="Q16" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="U16" s="1">
+        <v>0.51757707899077343</v>
+      </c>
+      <c r="V16" s="1"/>
+      <c r="Y16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z16" s="1">
+        <v>0.26820961398635512</v>
+      </c>
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>0.27706659</v>
       </c>
@@ -1550,8 +1785,22 @@
       <c r="Q17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+      <c r="T17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="U17" s="2">
+        <v>2.109815577833317</v>
+      </c>
+      <c r="V17" s="2"/>
+      <c r="Y17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z17" s="2">
+        <v>2.1009220402410378</v>
+      </c>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>0.73431679999999999</v>
       </c>
@@ -1601,7 +1850,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>5.3700350000000001E-2</v>
       </c>
@@ -1651,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>1.01997396</v>
       </c>
@@ -1701,7 +1950,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>1.8482500399999999</v>
       </c>
@@ -1751,7 +2000,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>0.82374561999999996</v>
       </c>
@@ -1801,7 +2050,7 @@
         <v>0.3333333</v>
       </c>
     </row>
-    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>0.27362692</v>
       </c>
@@ -1851,7 +2100,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>3.9690900000000001E-2</v>
       </c>
@@ -1901,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>1.5832008500000001</v>
       </c>
@@ -1951,7 +2200,7 @@
         <v>0.66666669999999995</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>0.49117488999999998</v>
       </c>
@@ -2001,7 +2250,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2070,7 +2319,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>0.19644865400312733</v>
       </c>
@@ -2120,8 +2369,7 @@
         <v>8.611111397849483E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2174,7 +2422,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>0.12663679999999999</v>
       </c>
@@ -2224,7 +2472,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>0.21096609999999999</v>
       </c>
@@ -2274,7 +2522,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>0.15335840000000001</v>
       </c>
@@ -2324,7 +2572,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>0.2202402</v>
       </c>
@@ -2374,7 +2622,7 @@
         <v>0.71428570000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>0.34585359999999998</v>
       </c>
@@ -2424,7 +2672,7 @@
         <v>0.57142859999999995</v>
       </c>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>0.1748159</v>
       </c>
@@ -2474,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B37">
         <v>0.21590039999999999</v>
       </c>
@@ -2524,7 +2772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>0.28717819999999999</v>
       </c>
@@ -2574,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39">
         <v>0.1841054</v>
       </c>
@@ -2624,7 +2872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40">
         <v>0.1727737</v>
       </c>
@@ -2674,7 +2922,7 @@
         <v>0.85714290000000004</v>
       </c>
     </row>
-    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>23</v>
       </c>
@@ -2743,7 +2991,7 @@
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B42">
         <v>2.0547654777695299E-2</v>
       </c>
@@ -2793,7 +3041,6 @@
         <v>4.4896104995469761E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>13</v>
@@ -3466,13 +3713,28 @@
         <v>5.7455169198194433E-2</v>
       </c>
     </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>36</v>
+      </c>
+      <c r="F57" t="s">
+        <v>42</v>
+      </c>
+      <c r="G57" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>36</v>
-      </c>
       <c r="E58">
         <f>(E2-E4)/SQRT(F4^2/10+F2^2/10)</f>
-        <v>-2.0897288898007078</v>
+        <v>-2.0897288898007096</v>
+      </c>
+      <c r="F58">
+        <f>(F2^2/10+F4^2/10)^2/((F2^2/10)^2/9+(F4^2/10)^2/9)</f>
+        <v>17.434395065172595</v>
+      </c>
+      <c r="G58">
+        <v>2.11</v>
       </c>
       <c r="I58">
         <f>(I2-I4)/SQRT(J4^2/10+J2^2/10)</f>
@@ -3501,6 +3763,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3509,7 +3772,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD12"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>